<commit_message>
Adjusted colors in stressor pie chart
</commit_message>
<xml_diff>
--- a/Data/sunburstplot_stressor.xlsx
+++ b/Data/sunburstplot_stressor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmajohnson/Desktop/Wong Lab/Review Paper/LitReviewGraphs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmajohnson/Desktop/Wong Lab/Review Paper/EmGePt_LitReview/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48124FED-394A-3946-ABB2-FF83BA696EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAD71D6-419E-F041-96B1-15130C71AB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35320" yWindow="160" windowWidth="27240" windowHeight="18900" xr2:uid="{BA3A640C-C91A-C442-822C-3A331EE9DB51}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{BA3A640C-C91A-C442-822C-3A331EE9DB51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>ids</t>
   </si>
@@ -59,49 +59,19 @@
     <t>Temperature</t>
   </si>
   <si>
-    <t>#00441b</t>
-  </si>
-  <si>
-    <t>#006d2c</t>
-  </si>
-  <si>
-    <t>#238b45</t>
-  </si>
-  <si>
     <t>pH</t>
-  </si>
-  <si>
-    <t>#41ab5d</t>
   </si>
   <si>
     <t>Pollution</t>
   </si>
   <si>
-    <t>#74c476</t>
-  </si>
-  <si>
     <t>Other</t>
-  </si>
-  <si>
-    <t>#a1d99b</t>
   </si>
   <si>
     <t>Hypoxia</t>
   </si>
   <si>
-    <t>#c7e9c0</t>
-  </si>
-  <si>
     <t>Salinity</t>
-  </si>
-  <si>
-    <t>#e5f5e0</t>
-  </si>
-  <si>
-    <t>#f7fcf5</t>
-  </si>
-  <si>
-    <t>#ffffff</t>
   </si>
   <si>
     <t>SSES</t>
@@ -150,6 +120,39 @@
   </si>
   <si>
     <t>Range &lt;br&gt;expansion&lt;br&gt;2% (5)</t>
+  </si>
+  <si>
+    <t>#003416</t>
+  </si>
+  <si>
+    <t>#DFF7E6</t>
+  </si>
+  <si>
+    <t>#F2FCF5</t>
+  </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>#005A22</t>
+  </si>
+  <si>
+    <t>#1E7A37</t>
+  </si>
+  <si>
+    <t>#3A9A4C</t>
+  </si>
+  <si>
+    <t>#64BC6B</t>
+  </si>
+  <si>
+    <t>#90D495</t>
+  </si>
+  <si>
+    <t>#BCECC2</t>
+  </si>
+  <si>
+    <t>#001F0E</t>
   </si>
 </sst>
 </file>
@@ -572,7 +575,7 @@
   <dimension ref="A1:J996"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,13 +607,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -624,13 +627,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="D3">
         <v>36</v>
@@ -647,10 +650,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
       </c>
       <c r="D4">
         <v>28</v>
@@ -664,13 +667,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
       </c>
       <c r="D5">
         <v>21</v>
@@ -684,13 +687,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -704,13 +707,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
       </c>
       <c r="D7">
         <v>18</v>
@@ -724,13 +727,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
       </c>
       <c r="D8">
         <v>18</v>
@@ -744,13 +747,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
       </c>
       <c r="D9">
         <v>13</v>
@@ -764,13 +767,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -784,13 +787,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
+      <c r="C11" t="s">
+        <v>30</v>
       </c>
       <c r="D11">
         <v>5</v>
@@ -804,13 +807,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -836,56 +839,67 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="D16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="D17" s="3"/>
+      <c r="F17" s="3"/>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="D18" s="3"/>
+      <c r="F18" s="3"/>
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="D19" s="3"/>
+      <c r="F19" s="3"/>
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="D20" s="3"/>
+      <c r="F20" s="3"/>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="D21" s="3"/>
+      <c r="F21" s="3"/>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="D22" s="3"/>
+      <c r="F22" s="3"/>
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="D23" s="3"/>
+      <c r="F23" s="3"/>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="D24" s="3"/>
+      <c r="F24" s="3"/>
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="D25" s="3"/>
+      <c r="F25" s="3"/>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="D26" s="3"/>
+      <c r="F26" s="3"/>
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>